<commit_message>
Added column, Alias, for tableau
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2021/ModelRuns_RTP2021.xlsx
+++ b/utilities/RTP/config_RTP2021/ModelRuns_RTP2021.xlsx
@@ -1,34 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A6999A-B1CA-452D-860D-928043490CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99F905B-94C3-4288-A08F-08AAB050B070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13695" yWindow="315" windowWidth="24300" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="0" windowWidth="25800" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$J$178</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="265">
   <si>
     <t>EEJ</t>
   </si>
@@ -805,6 +816,24 @@
   </si>
   <si>
     <t>BlueprintNetworks_64\net_2050_Alt2</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>2050 No Project</t>
+  </si>
+  <si>
+    <t>2050 EIR Alt1</t>
+  </si>
+  <si>
+    <t>2035 EIR Alt1</t>
+  </si>
+  <si>
+    <t>2035 EIR Alt2</t>
+  </si>
+  <si>
+    <t>2050 EIR Alt2</t>
   </si>
 </sst>
 </file>
@@ -1394,11 +1423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:J178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I178" sqref="I178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1409,9 +1438,10 @@
     <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="28" customWidth="1"/>
     <col min="9" max="9" width="49.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>40</v>
       </c>
@@ -1439,8 +1469,11 @@
       <c r="I1" s="45" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1460,8 +1493,9 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1481,8 +1515,9 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1502,8 +1537,9 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1523,8 +1559,9 @@
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1544,8 +1581,9 @@
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1565,8 +1603,9 @@
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -1586,8 +1625,9 @@
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -1607,8 +1647,9 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
@@ -1628,8 +1669,9 @@
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
@@ -1649,8 +1691,9 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1670,8 +1713,9 @@
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -1691,8 +1735,9 @@
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -1712,8 +1757,9 @@
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -1733,8 +1779,9 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1754,8 +1801,9 @@
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1775,8 +1823,9 @@
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
@@ -1796,8 +1845,9 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
@@ -1817,8 +1867,9 @@
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
@@ -1840,8 +1891,9 @@
         <v>220</v>
       </c>
       <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -1861,8 +1913,9 @@
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="s">
         <v>26</v>
       </c>
@@ -1888,8 +1941,9 @@
         <v>220</v>
       </c>
       <c r="I22" s="60"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="60"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1917,8 +1971,12 @@
       <c r="I23" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="2" t="str">
+        <f>TEXT(2015,"##")</f>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
@@ -1944,8 +2002,9 @@
         <v>43</v>
       </c>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
@@ -1969,8 +2028,9 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="50" t="s">
         <v>26</v>
       </c>
@@ -1994,8 +2054,9 @@
       </c>
       <c r="H26" s="64"/>
       <c r="I26" s="64"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="64"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
         <v>26</v>
       </c>
@@ -2019,8 +2080,9 @@
       </c>
       <c r="H27" s="62"/>
       <c r="I27" s="62"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="62"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>26</v>
       </c>
@@ -2044,8 +2106,9 @@
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -2071,8 +2134,9 @@
         <v>220</v>
       </c>
       <c r="I29" s="43"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>26</v>
       </c>
@@ -2100,8 +2164,12 @@
       <c r="I30" s="21" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="21" t="str">
+        <f>_xlfn.CONCAT(B30," ",E30)</f>
+        <v>2025 No Project</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>26</v>
       </c>
@@ -2125,8 +2193,9 @@
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>26</v>
       </c>
@@ -2152,8 +2221,9 @@
         <v>220</v>
       </c>
       <c r="I32" s="18"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="18"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="s">
         <v>26</v>
       </c>
@@ -2179,8 +2249,12 @@
         <v>43</v>
       </c>
       <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="31" t="str">
+        <f>_xlfn.CONCAT(B33," Plan")</f>
+        <v>2025 Plan</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="41" t="s">
         <v>26</v>
       </c>
@@ -2206,8 +2280,9 @@
         <v>220</v>
       </c>
       <c r="I34" s="43"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="43"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>26</v>
       </c>
@@ -2235,8 +2310,12 @@
       <c r="I35" s="21" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="21" t="str">
+        <f>_xlfn.CONCAT(B35," ",E35)</f>
+        <v>2030 No Project</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>26</v>
       </c>
@@ -2260,8 +2339,9 @@
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2287,8 +2367,9 @@
         <v>220</v>
       </c>
       <c r="I37" s="18"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>26</v>
       </c>
@@ -2312,8 +2393,9 @@
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="29" t="s">
         <v>26</v>
       </c>
@@ -2341,8 +2423,12 @@
       <c r="I39" s="31" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="31" t="str">
+        <f>_xlfn.CONCAT(B39," Plan")</f>
+        <v>2030 Plan</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>26</v>
       </c>
@@ -2362,8 +2448,9 @@
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>26</v>
       </c>
@@ -2383,8 +2470,9 @@
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
       <c r="I41" s="18"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>26</v>
       </c>
@@ -2404,8 +2492,9 @@
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>26</v>
       </c>
@@ -2431,8 +2520,9 @@
         <v>220</v>
       </c>
       <c r="I43" s="18"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="18"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>26</v>
       </c>
@@ -2460,8 +2550,9 @@
       <c r="I44" s="18" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>26</v>
       </c>
@@ -2481,8 +2572,9 @@
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="34"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>26</v>
       </c>
@@ -2502,8 +2594,9 @@
       <c r="G46" s="17"/>
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="18"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>26</v>
       </c>
@@ -2523,8 +2616,9 @@
       <c r="G47" s="17"/>
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="18"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>26</v>
       </c>
@@ -2544,8 +2638,9 @@
       <c r="G48" s="17"/>
       <c r="H48" s="18"/>
       <c r="I48" s="18"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>26</v>
       </c>
@@ -2569,8 +2664,9 @@
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="18"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>26</v>
       </c>
@@ -2594,8 +2690,9 @@
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="18"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
         <v>26</v>
       </c>
@@ -2619,8 +2716,9 @@
       </c>
       <c r="H51" s="31"/>
       <c r="I51" s="31"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="31"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="41" t="s">
         <v>26</v>
       </c>
@@ -2644,8 +2742,9 @@
       </c>
       <c r="H52" s="43"/>
       <c r="I52" s="43"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" s="43"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>26</v>
       </c>
@@ -2669,8 +2768,9 @@
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" s="15"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>26</v>
       </c>
@@ -2694,8 +2794,9 @@
       </c>
       <c r="H54" s="15"/>
       <c r="I54" s="15"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" s="15"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>26</v>
       </c>
@@ -2719,8 +2820,9 @@
       </c>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>26</v>
       </c>
@@ -2744,8 +2846,9 @@
       </c>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>26</v>
       </c>
@@ -2769,8 +2872,9 @@
       </c>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" s="15"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>26</v>
       </c>
@@ -2794,8 +2898,9 @@
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="15"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>26</v>
       </c>
@@ -2819,8 +2924,9 @@
       </c>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="15"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>26</v>
       </c>
@@ -2846,8 +2952,9 @@
         <v>220</v>
       </c>
       <c r="I60" s="15"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" s="15"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>26</v>
       </c>
@@ -2871,8 +2978,9 @@
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="15"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>26</v>
       </c>
@@ -2900,8 +3008,12 @@
       <c r="I62" s="21" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="21" t="str">
+        <f>_xlfn.CONCAT(B62," ",E62)</f>
+        <v>2035 No Project</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="32" t="s">
         <v>26</v>
       </c>
@@ -2921,8 +3033,9 @@
       <c r="G63" s="33"/>
       <c r="H63" s="34"/>
       <c r="I63" s="34"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" s="34"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="29" t="s">
         <v>26</v>
       </c>
@@ -2942,8 +3055,9 @@
       <c r="G64" s="30"/>
       <c r="H64" s="31"/>
       <c r="I64" s="31"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" s="31"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
         <v>26</v>
       </c>
@@ -2963,8 +3077,9 @@
       <c r="G65" s="17"/>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" s="18"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
         <v>26</v>
       </c>
@@ -2984,8 +3099,9 @@
       <c r="G66" s="17"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="18"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
         <v>26</v>
       </c>
@@ -3009,8 +3125,9 @@
       </c>
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" s="18"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
         <v>26</v>
       </c>
@@ -3034,8 +3151,9 @@
       </c>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" s="18"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
         <v>26</v>
       </c>
@@ -3059,8 +3177,9 @@
       </c>
       <c r="H69" s="18"/>
       <c r="I69" s="18"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" s="18"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>26</v>
       </c>
@@ -3084,8 +3203,9 @@
       </c>
       <c r="H70" s="18"/>
       <c r="I70" s="18"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="18"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>26</v>
       </c>
@@ -3109,8 +3229,9 @@
       </c>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="18"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>26</v>
       </c>
@@ -3136,8 +3257,9 @@
         <v>218</v>
       </c>
       <c r="I72" s="18"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="18"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
         <v>26</v>
       </c>
@@ -3161,8 +3283,9 @@
       </c>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="18"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
         <v>26</v>
       </c>
@@ -3186,8 +3309,9 @@
       </c>
       <c r="H74" s="18"/>
       <c r="I74" s="18"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" s="18"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
         <v>26</v>
       </c>
@@ -3211,8 +3335,9 @@
       </c>
       <c r="H75" s="18"/>
       <c r="I75" s="18"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="18"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
         <v>26</v>
       </c>
@@ -3236,8 +3361,9 @@
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="18"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="18"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>26</v>
       </c>
@@ -3261,8 +3387,9 @@
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="18"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="18"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>26</v>
       </c>
@@ -3286,8 +3413,9 @@
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="18"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="18"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="41" t="s">
         <v>26</v>
       </c>
@@ -3311,8 +3439,9 @@
       </c>
       <c r="H79" s="43"/>
       <c r="I79" s="43"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="43"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>26</v>
       </c>
@@ -3336,8 +3465,9 @@
       </c>
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80" s="15"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
         <v>26</v>
       </c>
@@ -3361,8 +3491,9 @@
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="15"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81" s="15"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>26</v>
       </c>
@@ -3386,8 +3517,9 @@
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="15"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82" s="15"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
         <v>26</v>
       </c>
@@ -3411,8 +3543,9 @@
       </c>
       <c r="H83" s="15"/>
       <c r="I83" s="15"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83" s="15"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>26</v>
       </c>
@@ -3436,8 +3569,9 @@
       </c>
       <c r="H84" s="15"/>
       <c r="I84" s="15"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84" s="15"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>26</v>
       </c>
@@ -3461,8 +3595,9 @@
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85" s="15"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>26</v>
       </c>
@@ -3486,8 +3621,9 @@
       </c>
       <c r="H86" s="15"/>
       <c r="I86" s="15"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86" s="15"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>26</v>
       </c>
@@ -3511,8 +3647,9 @@
       </c>
       <c r="H87" s="15"/>
       <c r="I87" s="15"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" s="15"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>26</v>
       </c>
@@ -3536,8 +3673,9 @@
       </c>
       <c r="H88" s="15"/>
       <c r="I88" s="15"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J88" s="15"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>26</v>
       </c>
@@ -3561,8 +3699,9 @@
       </c>
       <c r="H89" s="15"/>
       <c r="I89" s="15"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J89" s="15"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
         <v>26</v>
       </c>
@@ -3586,8 +3725,9 @@
       </c>
       <c r="H90" s="15"/>
       <c r="I90" s="15"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J90" s="15"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>26</v>
       </c>
@@ -3611,8 +3751,9 @@
       </c>
       <c r="H91" s="15"/>
       <c r="I91" s="15"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91" s="15"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
         <v>26</v>
       </c>
@@ -3636,8 +3777,9 @@
       </c>
       <c r="H92" s="15"/>
       <c r="I92" s="15"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J92" s="15"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
         <v>26</v>
       </c>
@@ -3663,8 +3805,9 @@
         <v>220</v>
       </c>
       <c r="I93" s="15"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93" s="15"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
         <v>26</v>
       </c>
@@ -3688,8 +3831,9 @@
       </c>
       <c r="H94" s="15"/>
       <c r="I94" s="15"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J94" s="15"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>26</v>
       </c>
@@ -3713,8 +3857,9 @@
       </c>
       <c r="H95" s="15"/>
       <c r="I95" s="15"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95" s="15"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
         <v>26</v>
       </c>
@@ -3738,8 +3883,9 @@
       </c>
       <c r="H96" s="15"/>
       <c r="I96" s="15"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96" s="15"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
         <v>26</v>
       </c>
@@ -3767,8 +3913,12 @@
       <c r="I97" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J97" s="21" t="str">
+        <f>_xlfn.CONCAT(B97," Plan")</f>
+        <v>2035 Plan</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="41" t="s">
         <v>26</v>
       </c>
@@ -3794,8 +3944,9 @@
         <v>220</v>
       </c>
       <c r="I98" s="43"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98" s="43"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
         <v>26</v>
       </c>
@@ -3823,8 +3974,12 @@
       <c r="I99" s="21" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99" s="21" t="str">
+        <f>_xlfn.CONCAT(B99," ",E99)</f>
+        <v>2040 No Project</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
         <v>26</v>
       </c>
@@ -3850,8 +4005,9 @@
         <v>220</v>
       </c>
       <c r="I100" s="43"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J100" s="43"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
         <v>26</v>
       </c>
@@ -3875,8 +4031,9 @@
       </c>
       <c r="H101" s="15"/>
       <c r="I101" s="15"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J101" s="15"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
         <v>26</v>
       </c>
@@ -3900,8 +4057,9 @@
       </c>
       <c r="H102" s="15"/>
       <c r="I102" s="15"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J102" s="15"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
         <v>26</v>
       </c>
@@ -3925,8 +4083,9 @@
       </c>
       <c r="H103" s="15"/>
       <c r="I103" s="15"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J103" s="15"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
         <v>26</v>
       </c>
@@ -3954,8 +4113,12 @@
       <c r="I104" s="21" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J104" s="21" t="str">
+        <f>_xlfn.CONCAT(B104," Plan")</f>
+        <v>2040 Plan</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="35" t="s">
         <v>26</v>
       </c>
@@ -3975,8 +4138,9 @@
       <c r="G105" s="26"/>
       <c r="H105" s="27"/>
       <c r="I105" s="27"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J105" s="27"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="25" t="s">
         <v>26</v>
       </c>
@@ -3996,8 +4160,9 @@
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
       <c r="I106" s="27"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J106" s="27"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
         <v>26</v>
       </c>
@@ -4021,8 +4186,9 @@
       </c>
       <c r="H107" s="27"/>
       <c r="I107" s="27"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J107" s="27"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="25" t="s">
         <v>26</v>
       </c>
@@ -4046,8 +4212,9 @@
       </c>
       <c r="H108" s="27"/>
       <c r="I108" s="27"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J108" s="27"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
         <v>26</v>
       </c>
@@ -4071,8 +4238,9 @@
       </c>
       <c r="H109" s="27"/>
       <c r="I109" s="27"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J109" s="27"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="25" t="s">
         <v>26</v>
       </c>
@@ -4096,8 +4264,9 @@
       </c>
       <c r="H110" s="27"/>
       <c r="I110" s="27"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J110" s="27"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="38" t="s">
         <v>26</v>
       </c>
@@ -4121,8 +4290,9 @@
       </c>
       <c r="H111" s="40"/>
       <c r="I111" s="40"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J111" s="40"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>26</v>
       </c>
@@ -4146,8 +4316,9 @@
       </c>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J112" s="15"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>26</v>
       </c>
@@ -4171,8 +4342,9 @@
       </c>
       <c r="H113" s="15"/>
       <c r="I113" s="15"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J113" s="15"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>26</v>
       </c>
@@ -4196,8 +4368,9 @@
       </c>
       <c r="H114" s="15"/>
       <c r="I114" s="15"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J114" s="15"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
         <v>26</v>
       </c>
@@ -4221,8 +4394,9 @@
       </c>
       <c r="H115" s="15"/>
       <c r="I115" s="15"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J115" s="15"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>26</v>
       </c>
@@ -4246,8 +4420,9 @@
       </c>
       <c r="H116" s="15"/>
       <c r="I116" s="15"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J116" s="15"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
         <v>26</v>
       </c>
@@ -4271,8 +4446,9 @@
       </c>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J117" s="15"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
         <v>26</v>
       </c>
@@ -4296,8 +4472,9 @@
       </c>
       <c r="H118" s="15"/>
       <c r="I118" s="15"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J118" s="15"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
         <v>26</v>
       </c>
@@ -4321,8 +4498,9 @@
       </c>
       <c r="H119" s="15"/>
       <c r="I119" s="15"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J119" s="15"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
         <v>26</v>
       </c>
@@ -4346,8 +4524,9 @@
       </c>
       <c r="H120" s="15"/>
       <c r="I120" s="15"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J120" s="15"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
         <v>26</v>
       </c>
@@ -4373,8 +4552,9 @@
         <v>220</v>
       </c>
       <c r="I121" s="15"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J121" s="15"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
         <v>26</v>
       </c>
@@ -4398,8 +4578,9 @@
       </c>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J122" s="15"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>26</v>
       </c>
@@ -4427,8 +4608,11 @@
       <c r="I123" s="21" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J123" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="25" t="s">
         <v>26</v>
       </c>
@@ -4448,8 +4632,9 @@
       <c r="G124" s="26"/>
       <c r="H124" s="27"/>
       <c r="I124" s="27"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J124" s="27"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="38" t="s">
         <v>26</v>
       </c>
@@ -4469,8 +4654,9 @@
       <c r="G125" s="39"/>
       <c r="H125" s="40"/>
       <c r="I125" s="40"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J125" s="40"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="25" t="s">
         <v>26</v>
       </c>
@@ -4490,8 +4676,9 @@
       <c r="G126" s="26"/>
       <c r="H126" s="27"/>
       <c r="I126" s="27"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J126" s="27"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="25" t="s">
         <v>26</v>
       </c>
@@ -4511,8 +4698,9 @@
       <c r="G127" s="26"/>
       <c r="H127" s="27"/>
       <c r="I127" s="27"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J127" s="27"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="25" t="s">
         <v>26</v>
       </c>
@@ -4536,8 +4724,9 @@
       </c>
       <c r="H128" s="27"/>
       <c r="I128" s="27"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J128" s="27"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="25" t="s">
         <v>26</v>
       </c>
@@ -4561,8 +4750,9 @@
       </c>
       <c r="H129" s="27"/>
       <c r="I129" s="27"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J129" s="27"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="25" t="s">
         <v>26</v>
       </c>
@@ -4586,8 +4776,9 @@
       </c>
       <c r="H130" s="27"/>
       <c r="I130" s="27"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J130" s="27"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="25" t="s">
         <v>26</v>
       </c>
@@ -4611,8 +4802,9 @@
       </c>
       <c r="H131" s="27"/>
       <c r="I131" s="27"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J131" s="27"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="25" t="s">
         <v>26</v>
       </c>
@@ -4636,8 +4828,9 @@
       </c>
       <c r="H132" s="27"/>
       <c r="I132" s="27"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J132" s="27"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="25" t="s">
         <v>26</v>
       </c>
@@ -4661,8 +4854,9 @@
       </c>
       <c r="H133" s="27"/>
       <c r="I133" s="27"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J133" s="27"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="25" t="s">
         <v>26</v>
       </c>
@@ -4688,8 +4882,9 @@
         <v>218</v>
       </c>
       <c r="I134" s="27"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J134" s="27"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="41" t="s">
         <v>26</v>
       </c>
@@ -4713,8 +4908,9 @@
       </c>
       <c r="H135" s="43"/>
       <c r="I135" s="43"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J135" s="43"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="13" t="s">
         <v>26</v>
       </c>
@@ -4738,8 +4934,9 @@
       </c>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J136" s="13"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
         <v>26</v>
       </c>
@@ -4763,8 +4960,9 @@
       </c>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J137" s="13"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>26</v>
       </c>
@@ -4788,8 +4986,9 @@
       </c>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J138" s="13"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>26</v>
       </c>
@@ -4813,8 +5012,9 @@
       </c>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J139" s="13"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
         <v>26</v>
       </c>
@@ -4838,8 +5038,9 @@
       </c>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J140" s="13"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
         <v>26</v>
       </c>
@@ -4863,8 +5064,9 @@
       </c>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J141" s="13"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>26</v>
       </c>
@@ -4888,8 +5090,9 @@
       </c>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J142" s="13"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>26</v>
       </c>
@@ -4913,8 +5116,9 @@
       </c>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J143" s="13"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>26</v>
       </c>
@@ -4938,8 +5142,9 @@
       </c>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J144" s="13"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>26</v>
       </c>
@@ -4963,8 +5168,9 @@
       </c>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J145" s="13"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>26</v>
       </c>
@@ -4988,8 +5194,9 @@
       </c>
       <c r="H146" s="15"/>
       <c r="I146" s="15"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J146" s="15"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>26</v>
       </c>
@@ -5013,8 +5220,9 @@
       </c>
       <c r="H147" s="15"/>
       <c r="I147" s="15"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J147" s="15"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>26</v>
       </c>
@@ -5038,8 +5246,9 @@
       </c>
       <c r="H148" s="15"/>
       <c r="I148" s="15"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J148" s="15"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>26</v>
       </c>
@@ -5063,8 +5272,9 @@
       </c>
       <c r="H149" s="15"/>
       <c r="I149" s="15"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J149" s="15"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
         <v>26</v>
       </c>
@@ -5088,8 +5298,9 @@
       </c>
       <c r="H150" s="15"/>
       <c r="I150" s="15"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J150" s="15"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
         <v>26</v>
       </c>
@@ -5113,8 +5324,9 @@
       </c>
       <c r="H151" s="15"/>
       <c r="I151" s="15"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J151" s="15"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
         <v>26</v>
       </c>
@@ -5138,8 +5350,9 @@
       </c>
       <c r="H152" s="15"/>
       <c r="I152" s="15"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J152" s="15"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>26</v>
       </c>
@@ -5163,8 +5376,9 @@
       </c>
       <c r="H153" s="15"/>
       <c r="I153" s="15"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J153" s="15"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
         <v>26</v>
       </c>
@@ -5188,8 +5402,9 @@
       </c>
       <c r="H154" s="15"/>
       <c r="I154" s="15"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J154" s="15"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
         <v>26</v>
       </c>
@@ -5215,8 +5430,9 @@
         <v>220</v>
       </c>
       <c r="I155" s="15"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J155" s="15"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
         <v>26</v>
       </c>
@@ -5240,8 +5456,9 @@
       </c>
       <c r="H156" s="15"/>
       <c r="I156" s="15"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J156" s="15"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
         <v>26</v>
       </c>
@@ -5265,8 +5482,9 @@
       </c>
       <c r="H157" s="15"/>
       <c r="I157" s="15"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J157" s="15"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="19" t="s">
         <v>26</v>
       </c>
@@ -5294,8 +5512,12 @@
       <c r="I158" s="21" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J158" s="21" t="str">
+        <f>_xlfn.CONCAT(B158," Plan")</f>
+        <v>2050 Plan</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="9" t="s">
         <v>26</v>
       </c>
@@ -5319,8 +5541,9 @@
       </c>
       <c r="H159" s="9"/>
       <c r="I159" s="9"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J159" s="9"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="9" t="s">
         <v>26</v>
       </c>
@@ -5344,8 +5567,9 @@
       </c>
       <c r="H160" s="9"/>
       <c r="I160" s="9"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J160" s="9"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="9" t="s">
         <v>26</v>
       </c>
@@ -5371,8 +5595,9 @@
         <v>220</v>
       </c>
       <c r="I161" s="9"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J161" s="9"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="9" t="s">
         <v>26</v>
       </c>
@@ -5396,8 +5621,9 @@
       </c>
       <c r="H162" s="9"/>
       <c r="I162" s="9"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J162" s="9"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
         <v>26</v>
       </c>
@@ -5421,8 +5647,9 @@
       </c>
       <c r="H163" s="9"/>
       <c r="I163" s="9"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J163" s="9"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="50" t="s">
         <v>26</v>
       </c>
@@ -5450,8 +5677,11 @@
       <c r="I164" s="50" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J164" s="50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="53" t="s">
         <v>26</v>
       </c>
@@ -5475,8 +5705,9 @@
       </c>
       <c r="H165" s="53"/>
       <c r="I165" s="53"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J165" s="53"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="9" t="s">
         <v>26</v>
       </c>
@@ -5500,8 +5731,9 @@
       </c>
       <c r="H166" s="9"/>
       <c r="I166" s="9"/>
-    </row>
-    <row r="167" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J166" s="9"/>
+    </row>
+    <row r="167" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="9" t="s">
         <v>26</v>
       </c>
@@ -5527,8 +5759,9 @@
         <v>220</v>
       </c>
       <c r="I167" s="9"/>
-    </row>
-    <row r="168" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J167" s="9"/>
+    </row>
+    <row r="168" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>26</v>
       </c>
@@ -5552,8 +5785,9 @@
       </c>
       <c r="H168" s="9"/>
       <c r="I168" s="9"/>
-    </row>
-    <row r="169" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J168" s="9"/>
+    </row>
+    <row r="169" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
         <v>26</v>
       </c>
@@ -5577,8 +5811,9 @@
       </c>
       <c r="H169" s="9"/>
       <c r="I169" s="9"/>
-    </row>
-    <row r="170" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J169" s="9"/>
+    </row>
+    <row r="170" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="50" t="s">
         <v>26</v>
       </c>
@@ -5606,8 +5841,11 @@
       <c r="I170" s="50" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J170" s="50" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="55" t="s">
         <v>26</v>
       </c>
@@ -5631,8 +5869,9 @@
       </c>
       <c r="H171" s="55"/>
       <c r="I171" s="55"/>
-    </row>
-    <row r="172" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J171" s="55"/>
+    </row>
+    <row r="172" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>26</v>
       </c>
@@ -5658,8 +5897,9 @@
         <v>220</v>
       </c>
       <c r="I172" s="6"/>
-    </row>
-    <row r="173" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J172" s="6"/>
+    </row>
+    <row r="173" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>26</v>
       </c>
@@ -5683,8 +5923,9 @@
       </c>
       <c r="H173" s="6"/>
       <c r="I173" s="6"/>
-    </row>
-    <row r="174" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J173" s="6"/>
+    </row>
+    <row r="174" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="57" t="s">
         <v>26</v>
       </c>
@@ -5712,8 +5953,11 @@
       <c r="I174" s="57" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J174" s="57" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
         <v>26</v>
       </c>
@@ -5737,8 +5981,9 @@
       </c>
       <c r="H175" s="6"/>
       <c r="I175" s="6"/>
-    </row>
-    <row r="176" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J175" s="6"/>
+    </row>
+    <row r="176" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="6" t="s">
         <v>26</v>
       </c>
@@ -5764,8 +6009,9 @@
         <v>220</v>
       </c>
       <c r="I176" s="6"/>
-    </row>
-    <row r="177" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J176" s="6"/>
+    </row>
+    <row r="177" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
         <v>26</v>
       </c>
@@ -5789,8 +6035,9 @@
       </c>
       <c r="H177" s="6"/>
       <c r="I177" s="6"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J177" s="6"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="6" t="s">
         <v>26</v>
       </c>
@@ -5818,8 +6065,12 @@
       <c r="I178" s="6" t="s">
         <v>258</v>
       </c>
+      <c r="J178" s="6" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J178" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>